<commit_message>
Before Adding the run metrics
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AF9880-11A2-424B-8274-AA1A1A11F99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD90A9D-AE16-467D-A056-C6DEA6508E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -276,12 +276,60 @@
      Reproduce the same behavior and logs from the CLI when triggered through GitHub
 This restructuring also had to preserve all existing features like:
      Extracting from multiple subreddits
-     Next page has no posts from yesterday     : ✅ Stop right away, print a message     
-     Next page has mixed days, only collect yesterday: ✅ Filter them, keep scraping         
-     Less than 500 posts available  : ✅ Accept fewer, no spillover from older days </t>
-  </si>
-  <si>
-    <t>Partially Completed</t>
+     Next page has no posts from yesterday
+     Next page has mixed days, only collect yesterday   
+     Less than 500 posts available  </t>
+  </si>
+  <si>
+    <t>23/7/2025(Onsite)</t>
+  </si>
+  <si>
+    <t>Partially Completed: The idempotency results or the main features and their idempotency errors needs extra checking
+Condition	                                                            Status	               Notes
+Extract from multiple subreddits	                               ✅ Fully Met	No issues.
+Stop when next page has no posts from yesterday	🟡 Partial	You filter, but don’t stop early. Add a check for all irrelevant posts.
+Only collect posts from yesterday if mixed days	 ✅ Fully Met	Correct filtering.
+Accept fewer than 500 posts, no older-day spillover	🟡 Partial	Filtering works, but no early exit when all new posts are too old.</t>
+  </si>
+  <si>
+    <t>Add debugging counters so that you can track the progress and the pressure that you apply on reddit's api</t>
+  </si>
+  <si>
+    <t>Test if the counters are working well when you change the t param from params dictionary from
+ week to day</t>
+  </si>
+  <si>
+    <t>24/7/2025(Vacation)</t>
+  </si>
+  <si>
+    <t>Modularize the Extractor code so that you can scale the project later on</t>
+  </si>
+  <si>
+    <t>DONE:
+day param output with the selected columns:
+=== Debugging Counters ===
+total_posts_fetched: 11792
+posts_filtered_time: 10855
+posts_filtered_comments: 41
+comments_skipped: 715
+valid_posts_stored: 665
+Completed in 15.40 minutes
+week param output with the selected columns:
+=== Debugging Counters ===
+total_posts_fetched: 11875
+posts_filtered_time: 10938
+posts_filtered_comments: 41
+comments_skipped: 715
+valid_posts_stored: 666
+Completed in 15.15 minutes
+Not that big of a difference, need to understand the underlying logic of the built in functions more. Currently at this stage I care about getting the MVP. Next step: automate the extraction process using prefect and github actions, then find a way to clean the unstructured textual columns in the extracted csv files.</t>
+  </si>
+  <si>
+    <t>25/7/2025(Vacation)</t>
+  </si>
+  <si>
+    <t>Make the script that will feed the data into The offline AI model and get its response and store it in 
+CSV file</t>
   </si>
 </sst>
 </file>
@@ -605,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR15"/>
+  <dimension ref="A1:CR19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +666,7 @@
     <col min="3" max="3" width="83.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="213.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="131.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="77.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="86.44140625" style="1" customWidth="1"/>
     <col min="7" max="95" width="8.88671875" style="1"/>
     <col min="97" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -901,8 +949,59 @@
       <c r="E15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wanted to go back to the working version: currently this code runs locally perfectly, hope the workflow works out too
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EEEF1D-6C51-47B4-B720-9D115DE310BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF5818C-A68A-41B8-B4F1-8AB2F62E4B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -349,6 +349,20 @@
   </si>
   <si>
     <t>DONE: deepseek model downloaded and will be used for the data cleaning</t>
+  </si>
+  <si>
+    <t>28/7/2025(Remote)</t>
+  </si>
+  <si>
+    <t>Try to make the prefect and the github actions to run the scripts daily without my need to run it 
+manually</t>
+  </si>
+  <si>
+    <t>While changing my code on a branch, the merged it into a the main branch by a mistake; therefore all of todays progression is gone. And I will have to 
+modularize the code again.</t>
+  </si>
+  <si>
+    <t>FAILED REALLY HARD</t>
   </si>
 </sst>
 </file>
@@ -672,9 +686,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR20"/>
+  <dimension ref="A1:CR21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="87" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="87" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1052,6 +1066,23 @@
         <v>75</v>
       </c>
     </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changing the work report
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF5818C-A68A-41B8-B4F1-8AB2F62E4B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBF9B84-587A-44E2-BAE1-7CD385E12B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -363,6 +363,39 @@
   </si>
   <si>
     <t>FAILED REALLY HARD</t>
+  </si>
+  <si>
+    <t>29/7/2025(Onsite)</t>
+  </si>
+  <si>
+    <t>Finding the right version of the code, although I added somehow good descriptive comment before each commit, need more descriptivness while writing 
+descriptions for each commit.</t>
+  </si>
+  <si>
+    <t>Recover the working version of the code.</t>
+  </si>
+  <si>
+    <t>Change the time of the autonomous extraction and test if it works on its own</t>
+  </si>
+  <si>
+    <t>Let the data be saved automatically into the data subdirectory in the main after each run</t>
+  </si>
+  <si>
+    <t>Start building the offline ai model that will clean the data in the data subdirectory then send it to a 
+new folder</t>
+  </si>
+  <si>
+    <t>Test the pipeline locally</t>
+  </si>
+  <si>
+    <t>DONE and the pipeline manual run on github is working perfectly الحمد الله
+The run took around 18 to 19 minutes to finish</t>
+  </si>
+  <si>
+    <t>The entry point in your code is run_pipeline.py from the main directory</t>
+  </si>
+  <si>
+    <t>DONE: The run took around 18 to 21 minutes</t>
   </si>
 </sst>
 </file>
@@ -686,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR21"/>
+  <dimension ref="A1:CR26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,6 +1116,73 @@
         <v>79</v>
       </c>
     </row>
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding new documents that describes the cleaner steps and logic
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBF9B84-587A-44E2-BAE1-7CD385E12B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F222DA-1430-413A-B544-3F848D2BC1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,9 +719,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR26"/>
+  <dimension ref="A1:CR27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="87" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="126" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1172,14 +1172,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the main to extract the latest csv file
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F222DA-1430-413A-B544-3F848D2BC1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1867CF2-7581-46F5-A5B5-5A14625D6FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -368,47 +368,105 @@
     <t>29/7/2025(Onsite)</t>
   </si>
   <si>
-    <t>Finding the right version of the code, although I added somehow good descriptive comment before each commit, need more descriptivness while writing 
-descriptions for each commit.</t>
-  </si>
-  <si>
-    <t>Recover the working version of the code.</t>
-  </si>
-  <si>
-    <t>Change the time of the autonomous extraction and test if it works on its own</t>
-  </si>
-  <si>
-    <t>Let the data be saved automatically into the data subdirectory in the main after each run</t>
-  </si>
-  <si>
-    <t>Start building the offline ai model that will clean the data in the data subdirectory then send it to a 
-new folder</t>
-  </si>
-  <si>
-    <t>Test the pipeline locally</t>
-  </si>
-  <si>
     <t>DONE and the pipeline manual run on github is working perfectly الحمد الله
 The run took around 18 to 19 minutes to finish</t>
   </si>
   <si>
-    <t>The entry point in your code is run_pipeline.py from the main directory</t>
-  </si>
-  <si>
     <t>DONE: The run took around 18 to 21 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Recover stable working version of the code</t>
+  </si>
+  <si>
+    <t>Identify and revert to the last working version of the pipeline</t>
+  </si>
+  <si>
+    <t>Although previous commits had descriptive messages, they lacked clarity. Improved commit discipline is needed.</t>
+  </si>
+  <si>
+    <t>Test the Reddit scraping pipeline locally</t>
+  </si>
+  <si>
+    <t>Use run_pipeline.py as the entry point from the main directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Schedule autonomous extraction via GitHub Actions</t>
+  </si>
+  <si>
+    <t>Configure the workflow to run automatically at 12:40 AM Egypt time</t>
+  </si>
+  <si>
+    <t>To validate correct UTC offset and time zone consistency</t>
+  </si>
+  <si>
+    <t>DONE   Confirmed: autonomous execution triggered on time.</t>
+  </si>
+  <si>
+    <t>30/7/2025(Onsite)</t>
+  </si>
+  <si>
+    <t>Save output data automatically to data/raw/</t>
+  </si>
+  <si>
+    <t>Ensure every autonomous or manual run writes results to data/raw/ subdirectory</t>
+  </si>
+  <si>
+    <t>Must ensure idempotency and avoid duplicate records across days</t>
+  </si>
+  <si>
+    <t>Begin building the offline AI model pipeline</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Develop a modular offline cleaning script to process </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>data/raw/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and save cleaned output to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>data/cleaned/</t>
+    </r>
+  </si>
+  <si>
+    <t>Will require I/O handling, LLM prompt formatting, and validation checks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -431,13 +489,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,13 +780,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR27"/>
+  <dimension ref="A1:CR26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="126" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="32.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.5546875" style="1" customWidth="1"/>
@@ -737,7 +798,7 @@
     <col min="97" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -757,7 +818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -777,7 +838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -797,7 +858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -814,7 +875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="12.6" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -834,7 +895,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -851,7 +912,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16.2" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -871,7 +932,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="19.2" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -891,7 +952,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -908,7 +969,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -925,7 +986,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="80.400000000000006" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -945,7 +1006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -959,7 +1020,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="129.6">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -979,7 +1040,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="100.8">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -999,7 +1060,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="172.8">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -1019,7 +1080,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28.8">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -1034,7 +1095,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="331.2">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -1048,7 +1109,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -1062,7 +1123,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="28.8">
       <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
@@ -1082,7 +1143,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -1099,7 +1160,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="28.8">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
@@ -1116,7 +1177,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="28.8">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
@@ -1124,16 +1185,19 @@
         <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>80</v>
       </c>
@@ -1143,14 +1207,14 @@
       <c r="C23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>88</v>
+      <c r="D23" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
@@ -1158,29 +1222,50 @@
         <v>15</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>85</v>
+        <v>93</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Ibrahim Hegazi Work Report and Issues.xlsx
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1867CF2-7581-46F5-A5B5-5A14625D6FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F9CFE8-D62D-4246-8F4B-93D41E202B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -449,6 +449,10 @@
   </si>
   <si>
     <t>Will require I/O handling, LLM prompt formatting, and validation checks</t>
+  </si>
+  <si>
+    <t>DONE: But the idempotency checks are not super complete yet, therefore we will check the ids of the 
+post in the upcoming phase before feeding the data to the offline ai model</t>
   </si>
 </sst>
 </file>
@@ -782,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="88" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1234,7 +1238,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="28.8">
       <c r="A25" s="1" t="s">
         <v>92</v>
       </c>
@@ -1249,6 +1253,9 @@
       </c>
       <c r="E25" s="1" t="s">
         <v>95</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:6">

</xml_diff>

<commit_message>
Reverting a change that i made in the workflow file
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F9CFE8-D62D-4246-8F4B-93D41E202B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F79FA28-916D-4A81-B548-9229920B760E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>Date</t>
   </si>
@@ -400,9 +400,6 @@
   </si>
   <si>
     <t>DONE   Confirmed: autonomous execution triggered on time.</t>
-  </si>
-  <si>
-    <t>30/7/2025(Onsite)</t>
   </si>
   <si>
     <t>Save output data automatically to data/raw/</t>
@@ -453,6 +450,41 @@
   <si>
     <t>DONE: But the idempotency checks are not super complete yet, therefore we will check the ids of the 
 post in the upcoming phase before feeding the data to the offline ai model</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Partially Done: Initial architecture planned and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>flow.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> structure drafted</t>
+    </r>
+  </si>
+  <si>
+    <t>30/7/2025(Remote)</t>
+  </si>
+  <si>
+    <t>Make a GitHub branch and structure the directories as planned</t>
+  </si>
+  <si>
+    <t>You will need to test the old pipeline before making any modifications</t>
+  </si>
+  <si>
+    <t>Check how the medical o1 data set looked like so that you can format your data set in the same way</t>
   </si>
 </sst>
 </file>
@@ -784,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR26"/>
+  <dimension ref="A1:CR28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="185" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1240,39 +1272,67 @@
     </row>
     <row r="25" spans="1:6" ht="28.8">
       <c r="A25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>98</v>
+      <c r="F26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding more needed documentations and time plan, and started implementing The testing version of the cleaner LLM
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F79FA28-916D-4A81-B548-9229920B760E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDFE0F7-838C-4B49-BEA7-89D86E31DF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -409,9 +409,6 @@
   </si>
   <si>
     <t>Must ensure idempotency and avoid duplicate records across days</t>
-  </si>
-  <si>
-    <t>Begin building the offline AI model pipeline</t>
   </si>
   <si>
     <r>
@@ -448,10 +445,6 @@
     <t>Will require I/O handling, LLM prompt formatting, and validation checks</t>
   </si>
   <si>
-    <t>DONE: But the idempotency checks are not super complete yet, therefore we will check the ids of the 
-post in the upcoming phase before feeding the data to the offline ai model</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Partially Done: Initial architecture planned and </t>
     </r>
@@ -485,6 +478,35 @@
   </si>
   <si>
     <t>Check how the medical o1 data set looked like so that you can format your data set in the same way</t>
+  </si>
+  <si>
+    <t>Improve the file structure and readme file to include all the needed phases.</t>
+  </si>
+  <si>
+    <t>DONE: Old pipeline tested and worked perfectly, and the new branch is created for phase two</t>
+  </si>
+  <si>
+    <t>Make the super comprehensive roadmap for the full project</t>
+  </si>
+  <si>
+    <t>Generate a fake meta data for the branches so that you can test with later on</t>
+  </si>
+  <si>
+    <t>Know the inputs and outputs of each phase and what happens at each phase</t>
+  </si>
+  <si>
+    <t>After making 3 roadmaps combine the needed parts: Combine 3 ROADMAPS and FILE STRUTURES and MindMaps</t>
+  </si>
+  <si>
+    <t>DONE: But the idempotency checks are not super complete yet, therefore we will check the ids of the 
+post in the upcoming phase before feeding the data to the offline ai model.
+Before AI processing, introduce a lightweight deduplication mechanism (e.g., store post_id, scraped_at in metadata).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begin building the offline AI model pipeline </t>
+  </si>
+  <si>
+    <t>31/7/2025(Onsite)</t>
   </si>
 </sst>
 </file>
@@ -816,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR28"/>
+  <dimension ref="A1:CR32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="185" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="103" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1270,9 +1292,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28.8">
+    <row r="25" spans="1:6" ht="57.6">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>15</v>
@@ -1287,52 +1309,105 @@
         <v>94</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" t="s">
         <v>97</v>
-      </c>
-      <c r="F26" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>102</v>
+      <c r="F27" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating some research files
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDFE0F7-838C-4B49-BEA7-89D86E31DF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3889CA-0F2B-4588-944D-6CFE6C2A1B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="118">
   <si>
     <t>Date</t>
   </si>
@@ -507,6 +507,29 @@
   </si>
   <si>
     <t>31/7/2025(Onsite)</t>
+  </si>
+  <si>
+    <t>Design a Comprehensive Execution Plan for the LLM Cleaner (Phase 2)</t>
+  </si>
+  <si>
+    <t>While reviewing the existing roadmap, I found it provides a solid high-level direction but lacks actionable detail on how to execute the offline LLM cleaning pipeline—particularly how it integrates with GitHub workflows. Today’s focus was to fill in those missing specifics.</t>
+  </si>
+  <si>
+    <t>A key challenge emerged when attempting to upload the quantized LLM model to GitHub to enable a fully online workflow. GitHub’s file size limits and runner 
+constraints made this infeasible. This broke the assumption that the entire pipeline could run in the cloud autonomously, revealing the need for an 
+offline/hybrid execution path that would rely on my device being powered on at certain steps.</t>
+  </si>
+  <si>
+    <t>1/8/2025(Vacation)</t>
+  </si>
+  <si>
+    <t>Write the script that will download the model locally</t>
+  </si>
+  <si>
+    <t>DONE: The code has been written and the model has been downloaded</t>
+  </si>
+  <si>
+    <t>DONE: The folder explaining this point is stored at Car_Clinic_Project/docs/Project Understanding Questions.docx</t>
   </si>
 </sst>
 </file>
@@ -838,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR32"/>
+  <dimension ref="A1:CR40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="103" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="103" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -851,7 +874,7 @@
     <col min="3" max="3" width="83.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="213.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="131.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="86.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="104.109375" style="1" customWidth="1"/>
     <col min="7" max="95" width="8.88671875" style="1"/>
     <col min="97" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1366,7 +1389,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" ht="57.6">
       <c r="A29" s="1" t="s">
         <v>110</v>
       </c>
@@ -1374,7 +1397,13 @@
         <v>15</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1385,7 +1414,10 @@
         <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>115</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1396,18 +1428,43 @@
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commiting the github action cleaner that uses ollama
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3889CA-0F2B-4588-944D-6CFE6C2A1B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8395B7E-DE08-4AE7-8629-A9AEF3764CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="124">
   <si>
     <t>Date</t>
   </si>
@@ -530,6 +530,26 @@
   </si>
   <si>
     <t>DONE: The folder explaining this point is stored at Car_Clinic_Project/docs/Project Understanding Questions.docx</t>
+  </si>
+  <si>
+    <t>2/8/2025(Remote)</t>
+  </si>
+  <si>
+    <t>Search more about together ai and how to implement it in the pipeline</t>
+  </si>
+  <si>
+    <t>After downloading the offline ai model and finishing the initial script, the script took 2 minutes for each row. And we have approcimately 10 folders, each containing around 600 rows; therefore, the amount of time needed to clean that data Is tremendous.
+ Therefore, i tried to look for alternatives.</t>
+  </si>
+  <si>
+    <t>DONE: The search session is done, the same issue as before no free model that can handle the needed amount of data and
+I don’t want to waste time on a limit platform accesses</t>
+  </si>
+  <si>
+    <t>Search more about free ai apis to get this unstructured data</t>
+  </si>
+  <si>
+    <t>DONE: the possible options are Kaggle notebooks, Ollama in Github actions, Hugging face inference api, and lots of paid options</t>
   </si>
 </sst>
 </file>
@@ -861,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CR40"/>
+  <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="103" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="77" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1176,7 +1196,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="331.2">
+    <row r="17" spans="1:6" ht="316.8">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -1315,7 +1335,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="57.6">
+    <row r="25" spans="1:6" ht="43.2">
       <c r="A25" s="1" t="s">
         <v>98</v>
       </c>
@@ -1434,36 +1454,67 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
+    <row r="32" spans="1:6" ht="28.8">
+      <c r="A32" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B101" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
+    <row r="102" spans="1:3">
+      <c r="A102" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B102" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B103" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Showing the prompt before it goes to the model
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF269F80-1772-4EEE-9737-63EE04FF8AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C921A6EC-A6A7-4049-B557-13784C55C8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="142">
   <si>
     <t>Date</t>
   </si>
@@ -678,6 +678,15 @@
     Diagnosed that the issue stemmed from booting the model for each row.
     Decided to switch to ollama-python client with a persistent local server (hosted on http://localhost:11434).
     Implemented the Client.chat() method for 10x+ faster row-by-row inference.</t>
+  </si>
+  <si>
+    <t>4/8/2025(Remote)</t>
+  </si>
+  <si>
+    <t>Add the code that shows the prompt before sending it to the model</t>
+  </si>
+  <si>
+    <t>Check if there are any errors related to the json going in or out of the model</t>
   </si>
 </sst>
 </file>
@@ -1031,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F51" sqref="F47:F51"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1728,7 +1737,30 @@
       </c>
     </row>
     <row r="40" spans="1:6">
+      <c r="A40" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="E40" s="7"/>
+      <c r="F40" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">

</xml_diff>

<commit_message>
Updated How the json sent works
The error that made me look at the code for 2 days was that i forgot the 's' in top_comments
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C921A6EC-A6A7-4049-B557-13784C55C8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E9F125-D3C7-4BA0-B8B2-3E771ED9FE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2784" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1040,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
WORKING VERSION OF LLM CLEANER THAT NEEDS TO BE SCALED UP
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E9F125-D3C7-4BA0-B8B2-3E771ED9FE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CA93FC-4697-4188-9315-3B6B19F74804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2784" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="153">
   <si>
     <t>Date</t>
   </si>
@@ -687,6 +687,40 @@
   </si>
   <si>
     <t>Check if there are any errors related to the json going in or out of the model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used logger.info to print the prompt per row for debugging and analysis </t>
+  </si>
+  <si>
+    <t>Investigated JSONDecodeError; confirmed cause was due to me writing the top_comments column name wrong by forgetting the 's' at the end of it</t>
+  </si>
+  <si>
+    <t>Review quality of extracted content from LLM</t>
+  </si>
+  <si>
+    <t>Manually reviewed several rows; evaluated clarity, correctness, and usability of output</t>
+  </si>
+  <si>
+    <t>Not statisfied with the output, I feel that lots of the needed context for the diagnosis is missing from the main extracted data</t>
+  </si>
+  <si>
+    <t>DONE: Prompt engineering task incoming but after finding a scalable solution for the upcoming problem</t>
+  </si>
+  <si>
+    <t>Measure total time taken for batch processing</t>
+  </si>
+  <si>
+    <t>DONE: 44 rows took ~2 hours; extrapolated daily 700 rows to ~31.3 hours. NEEDS A SCALABLE SOLUTION INSTEAD OF 
+GITHUB ACTIONS LLMS</t>
+  </si>
+  <si>
+    <t>Improve the loggings even more to identify where are the bottlenecks</t>
+  </si>
+  <si>
+    <t>The process was going smoothly until I had to Remove all the changes that I have made today to an older working version of the branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAILED REALLY HARD due to not testing comprhensively and waiting for the output cleaned file to see the formatting </t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1746,6 +1780,9 @@
       <c r="C40" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="D40" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="E40" s="7"/>
       <c r="F40" s="1" t="s">
         <v>36</v>
@@ -1759,7 +1796,64 @@
         <v>15</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>141</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8">
+      <c r="A44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:3">

</xml_diff>

<commit_message>
Downloading OBD codes dataset
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CA93FC-4697-4188-9315-3B6B19F74804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5308664F-3CC0-41F0-B08B-A09B12D3B716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="156">
   <si>
     <t>Date</t>
   </si>
@@ -721,6 +721,15 @@
   </si>
   <si>
     <t xml:space="preserve">FAILED REALLY HARD due to not testing comprhensively and waiting for the output cleaned file to see the formatting </t>
+  </si>
+  <si>
+    <t>5/8/2025(Remote)</t>
+  </si>
+  <si>
+    <t>Search for an automation expert to help u find a solution for your problem.</t>
+  </si>
+  <si>
+    <t>DONE: https://www.linkedin.com/in/sherin-bassem-4a2b14372/      , Wating for his reply</t>
   </si>
 </sst>
 </file>
@@ -1074,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="E39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1856,6 +1865,20 @@
         <v>149</v>
       </c>
     </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Adding new extra scripts while saying good bye for this project until i get money or until i get into unethical automation
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5308664F-3CC0-41F0-B08B-A09B12D3B716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC630EB-21EC-4309-A259-A2BB9BAE5B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="160">
   <si>
     <t>Date</t>
   </si>
@@ -730,6 +730,20 @@
   </si>
   <si>
     <t>DONE: https://www.linkedin.com/in/sherin-bassem-4a2b14372/      , Wating for his reply</t>
+  </si>
+  <si>
+    <t>6/8/2025(Onsite)</t>
+  </si>
+  <si>
+    <t>Track the response of the expert that you talked to</t>
+  </si>
+  <si>
+    <t>DONE: He provided resources for more advanced scraping techniques but he didn’t help me for better overall
+automation for my problem Current issue</t>
+  </si>
+  <si>
+    <t>Formalize the problem statement and its possible solutions and the cost specifications for
+these solutions, so that the final document will be sent to the stakeholders.</t>
   </si>
 </sst>
 </file>
@@ -1083,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1879,6 +1893,34 @@
         <v>155</v>
       </c>
     </row>
+    <row r="46" spans="1:6" ht="28.8">
+      <c r="A46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.8">
+      <c r="A47" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Making the Cleaner Code clean 10 rows for testing purposes
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE53F15E-057B-47E7-B8B1-B6E988ECD784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E172FD8-7181-46F3-ABE3-FBB2EF482440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="164">
   <si>
     <t>Date</t>
   </si>
@@ -751,6 +751,16 @@
   <si>
     <t>Modify the code to clean only 10 rows instead of the whole dataset to see if the code saves the
  cleaned data in the needed way and in the right folder</t>
+  </si>
+  <si>
+    <t>Modularize the LLM Cleaner Code</t>
+  </si>
+  <si>
+    <t>Finalize the Readme file and don’t forget to add the following:
+1)Competitors
+2)Where I stopped in the phases of the project
+3)What was the issue
+4)Suggested Solutions</t>
   </si>
 </sst>
 </file>
@@ -1104,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1939,6 +1949,28 @@
         <v>161</v>
       </c>
     </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="72">
+      <c r="A50" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Pre testing the modularized version of the LLM cleaner
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E172FD8-7181-46F3-ABE3-FBB2EF482440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB3699D-27D3-44BF-8E5A-286A59129032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="168">
   <si>
     <t>Date</t>
   </si>
@@ -761,6 +761,18 @@
 2)Where I stopped in the phases of the project
 3)What was the issue
 4)Suggested Solutions</t>
+  </si>
+  <si>
+    <t>Remember to change the extraction and limit rate to the normal</t>
+  </si>
+  <si>
+    <t>Make LinkedIn Post</t>
+  </si>
+  <si>
+    <t>دراسة جدوى</t>
+  </si>
+  <si>
+    <t>secret env variab;es</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1948,6 +1960,9 @@
       <c r="C48" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="F48" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
@@ -1969,6 +1984,38 @@
       </c>
       <c r="C50" s="2" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="C53" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="C54" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="101" spans="1:3">

</xml_diff>

<commit_message>
Added the Reddit Post ID to the cleaned data so that we can apply the idempotency rule that i mentioned previously in the Work Report
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB3699D-27D3-44BF-8E5A-286A59129032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B296D48-CD4C-46F5-B418-B236B0871305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="169">
   <si>
     <t>Date</t>
   </si>
@@ -773,6 +773,10 @@
   </si>
   <si>
     <t>secret env variab;es</t>
+  </si>
+  <si>
+    <t>Add the reddit post id, so that later on you can apply the idempotency rule that you mentioned
+previously</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1131,7 @@
   <dimension ref="A1:CR103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2018,6 +2022,11 @@
         <v>167</v>
       </c>
     </row>
+    <row r="55" spans="1:3" ht="28.8">
+      <c r="C55" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Modifying the secret stuff
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B296D48-CD4C-46F5-B418-B236B0871305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAE91C1-E4DD-49D4-B9A7-B68F5A9C94C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="169">
   <si>
     <t>Date</t>
   </si>
@@ -763,20 +763,21 @@
 4)Suggested Solutions</t>
   </si>
   <si>
-    <t>Remember to change the extraction and limit rate to the normal</t>
-  </si>
-  <si>
     <t>Make LinkedIn Post</t>
   </si>
   <si>
     <t>دراسة جدوى</t>
-  </si>
-  <si>
-    <t>secret env variab;es</t>
   </si>
   <si>
     <t>Add the reddit post id, so that later on you can apply the idempotency rule that you mentioned
 previously</t>
+  </si>
+  <si>
+    <t>secret env variables</t>
+  </si>
+  <si>
+    <t>Remember to change the extraction and limit rate to the normal AND remove any emojis from 
+your code base</t>
   </si>
 </sst>
 </file>
@@ -1130,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1968,7 +1969,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
         <v>160</v>
       </c>
@@ -1978,8 +1979,11 @@
       <c r="C49" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="72">
+      <c r="F49" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="72">
       <c r="A50" s="1" t="s">
         <v>160</v>
       </c>
@@ -1990,18 +1994,18 @@
         <v>163</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:6" ht="28.8">
       <c r="A51" s="1" t="s">
         <v>160</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="C51" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
         <v>160</v>
       </c>
@@ -2009,22 +2013,43 @@
         <v>15</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="C53" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:6">
+      <c r="A54" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C54" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="28.8">
+    <row r="55" spans="1:6" ht="28.8">
+      <c r="A55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C55" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="101" spans="1:3">

</xml_diff>

<commit_message>
Modifying the comments cleaner and removing the reddits secrets
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAE91C1-E4DD-49D4-B9A7-B68F5A9C94C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7503E-89F4-4CA7-AA6C-F76AD0A088E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="169">
   <si>
     <t>Date</t>
   </si>
@@ -1131,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2037,6 +2037,9 @@
       <c r="C54" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="F54" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="28.8">
       <c r="A55" s="1" t="s">

</xml_diff>

<commit_message>
Add the system architecture diagram
</commit_message>
<xml_diff>
--- a/docs/Ibrahim Hegazi Work Report and Issues.xlsx
+++ b/docs/Ibrahim Hegazi Work Report and Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\Eagles\Car_Clinic_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05161EF-B27C-42CA-85D5-098E2F50B5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34634143-25DC-4D85-99FA-40B9B80F2E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="171">
   <si>
     <t>Date</t>
   </si>
@@ -777,6 +777,12 @@
   </si>
   <si>
     <t>Remember to change the extraction and limit rate to the normal</t>
+  </si>
+  <si>
+    <t>Merge the branches and test if the main branch is working perfectly</t>
+  </si>
+  <si>
+    <t>9/8/2025(Remote)</t>
   </si>
 </sst>
 </file>
@@ -1130,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2057,6 +2063,20 @@
         <v>36</v>
       </c>
     </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
         <v>114</v>

</xml_diff>